<commit_message>
Changed SHA1 generator flow
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Afzal_Shaikh\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Settings" sheetId="1" r:id="rId1"/>
-    <sheet name="Constants" sheetId="2" r:id="rId2"/>
-    <sheet name="Assets" sheetId="3" r:id="rId3"/>
+    <sheet name="Settings" sheetId="1" r:id="rId3"/>
+    <sheet name="Constants" sheetId="2" r:id="rId4"/>
+    <sheet name="Email" sheetId="4" r:id="rId5"/>
+    <sheet name="Assets" sheetId="3" r:id="rId6"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="85">
   <si>
     <t>Name</t>
   </si>
@@ -91,15 +92,12 @@
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
@@ -160,23 +158,218 @@
   </si>
   <si>
     <t>ProcessABCQueue</t>
+  </si>
+  <si>
+    <t>Bot has encounter an unhandle exception.
+****This is a system generated email, do not reply to this email.****</t>
+  </si>
+  <si>
+    <t>theafzalshaikh@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Failed : Calculate Client Security Hash Process | </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Success : Calculate Client Security Hash Process | </t>
+  </si>
+  <si>
+    <t>Calculate client security hash process executed successfully.
+****This is a system generated email, do not reply to this email.****</t>
+  </si>
+  <si>
+    <t>AcmeSystem1Credentials</t>
+  </si>
+  <si>
+    <t>TOAddress</t>
+  </si>
+  <si>
+    <t>CCAddress</t>
+  </si>
+  <si>
+    <t>CCSHTOAddress</t>
+  </si>
+  <si>
+    <t>CCSHCCAddress</t>
+  </si>
+  <si>
+    <t>AcmeSystem1LoginPageURL</t>
+  </si>
+  <si>
+    <t>SHA1LoginPageURL</t>
+  </si>
+  <si>
+    <t>AcmeSystem1DashboardPageURL</t>
+  </si>
+  <si>
+    <t>AcmeSystem1WorkItemPageURL</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/login</t>
+  </si>
+  <si>
+    <t>https://codebeautify.org/sha1-hash-generator/</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/work-items/</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/</t>
+  </si>
+  <si>
+    <t>Body_UnhandleException</t>
+  </si>
+  <si>
+    <t>Body_Success</t>
+  </si>
+  <si>
+    <t>Subject_Failure</t>
+  </si>
+  <si>
+    <t>Subject_Success</t>
+  </si>
+  <si>
+    <t>OutlookAccount</t>
+  </si>
+  <si>
+    <t>Body_ACMESystemWrongCredentials</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ACME System1 wrong credentials.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>****It is a computer generated email, and you should not reply to it.****</t>
+    </r>
+  </si>
+  <si>
+    <t>Body_ACMESystemLoginPageNotResponding</t>
+  </si>
+  <si>
+    <t>Body_ACMESystemHomePageNotResponding</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ACME System1 portal home page is not displayed.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>****It is a computer generated email, and you should not reply to it.****</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ACME System1 portal login page prompting username &amp; password is not displayed.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>****It is a computer generated email, and you should not reply to it.****</t>
+    </r>
+  </si>
+  <si>
+    <t>Body_ACMESystemUnableToNavigateWorkItemsPage</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ACME System1 unable to navigate on work items page
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>****It is a computer generated email, and you should not reply to it.****</t>
+    </r>
+  </si>
+  <si>
+    <t>Body_SHA1HomePageNotResponding</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SHA1 portal home page is not displayed.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>****It is a computer generated email, and you should not reply to it.****</t>
+    </r>
+  </si>
+  <si>
+    <t>LogFileFolder</t>
+  </si>
+  <si>
+    <t>LogFileName</t>
+  </si>
+  <si>
+    <t>Logs</t>
+  </si>
+  <si>
+    <t>D:\UiPath\Calculate Client Security Hash\Data\Logs\</t>
+  </si>
+  <si>
+    <t>D:\UiPath\Calculate Client Security Hash\Exceptions_Screenshots\</t>
+  </si>
+  <si>
+    <t>ExceptionScreenshotFolderPath</t>
+  </si>
+  <si>
+    <t>Hi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="6"/>
@@ -185,6 +378,7 @@
       <charset val="128"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -208,25 +402,137 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="15" builtinId="5"/>
+    <cellStyle name="Currency" xfId="16" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
+    <cellStyle name="Comma" xfId="18" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -534,19 +840,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.424285714285714" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.57142857142857" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.42857142857143" customWidth="1"/>
+    <col min="4" max="26" width="8.714285714285714" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -583,7 +889,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+    <row r="2" spans="1:3" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
@@ -594,7 +900,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:3" ht="45">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -603,8 +909,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="4" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:3" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -615,17 +921,70 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" ht="14.25" customHeight="1">
+      <c r="B15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -1607,28 +1966,26 @@
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z988"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0" topLeftCell="A11">
+      <selection pane="topLeft" activeCell="B27" sqref="B27:B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.424285714285714" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42857142857143" customWidth="1"/>
+    <col min="4" max="26" width="8.714285714285714" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1665,7 +2022,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:3" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1676,7 +2033,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:3" ht="45">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1687,8 +2044,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+    <row r="4" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:3" ht="14.25" customHeight="1">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1699,8 +2056,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+    <row r="6" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:3" ht="14.25" customHeight="1">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1711,7 +2068,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+    <row r="8" spans="1:3" ht="14.25" customHeight="1">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1722,7 +2079,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+    <row r="9" spans="1:3" ht="14.25" customHeight="1">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1733,7 +2090,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+    <row r="10" spans="1:3" ht="14.25" customHeight="1">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1744,7 +2101,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+    <row r="11" spans="1:3" ht="14.25" customHeight="1">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1755,7 +2112,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+    <row r="12" spans="1:3" ht="14.25" customHeight="1">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1766,8 +2123,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+    <row r="13" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:3" ht="14.25" customHeight="1">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1778,7 +2135,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+    <row r="15" spans="1:3" ht="14.25" customHeight="1">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -1789,8 +2146,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="16" ht="14.25" customHeight="1"/>
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -1801,21 +2158,21 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="18" ht="14.25" customHeight="1"/>
+    <row r="19" ht="14.25" customHeight="1"/>
+    <row r="20" ht="14.25" customHeight="1"/>
+    <row r="21" ht="14.25" customHeight="1"/>
+    <row r="22" ht="14.25" customHeight="1"/>
+    <row r="23" ht="14.25" customHeight="1"/>
+    <row r="24" ht="14.25" customHeight="1"/>
+    <row r="25" ht="14.25" customHeight="1"/>
+    <row r="26" ht="14.25" customHeight="1"/>
+    <row r="27" ht="14.25" customHeight="1"/>
+    <row r="28" ht="14.25" customHeight="1"/>
+    <row r="29" ht="14.25" customHeight="1"/>
+    <row r="30" ht="14.25" customHeight="1"/>
+    <row r="31" ht="14.25" customHeight="1"/>
+    <row r="32" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -2773,23 +3130,136 @@
     <row r="987" ht="14.25" customHeight="1"/>
     <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z1000"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCAEE62C-CE78-434B-A9A5-C9B7331DBD4E}">
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="30.428571428571427" style="7" customWidth="1"/>
+    <col min="2" max="2" width="37.57142857142857" style="7" customWidth="1"/>
+    <col min="3" max="3" width="21.857142857142858" style="7" customWidth="1"/>
+    <col min="4" max="16384" width="9.142857142857142" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15">
+      <c r="A2" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15">
+      <c r="A3" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15">
+      <c r="A4" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="75">
+      <c r="A5" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="75">
+      <c r="A6" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="90">
+      <c r="A7" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="60">
+      <c r="A8" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="75">
+      <c r="A9" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="75">
+      <c r="A10" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="60">
+      <c r="A11" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:Z4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.424285714285714" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="31.857142857142858" customWidth="1"/>
+    <col min="2" max="2" width="30.142857142857142" customWidth="1"/>
+    <col min="3" max="3" width="60.285714285714285" customWidth="1"/>
+    <col min="4" max="26" width="65.42857142857143" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2828,21 +3298,42 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25" customHeight="1"/>
+    <row r="6" ht="14.25" customHeight="1"/>
+    <row r="7" ht="14.25" customHeight="1"/>
+    <row r="8" ht="14.25" customHeight="1"/>
+    <row r="9" ht="14.25" customHeight="1"/>
+    <row r="10" ht="14.25" customHeight="1"/>
+    <row r="11" ht="14.25" customHeight="1"/>
+    <row r="12" ht="14.25" customHeight="1"/>
+    <row r="13" ht="14.25" customHeight="1"/>
+    <row r="14" ht="14.25" customHeight="1"/>
+    <row r="15" ht="14.25" customHeight="1"/>
+    <row r="16" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -3828,7 +4319,6 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>